<commit_message>
ZSS-1072 The font "Calibri" is missing from the dropdown in the toolbar
</commit_message>
<xml_diff>
--- a/zssapp/src/archive/web/zssapp/blank.xlsx
+++ b/zssapp/src/archive/web/zssapp/blank.xlsx
@@ -1,35 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="17040" windowHeight="11280" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="新細明體"/>
-      <family val="2"/>
-      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -51,14 +43,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,13 +343,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -370,13 +355,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>